<commit_message>
call func write test result order to excel
</commit_message>
<xml_diff>
--- a/at_amazon/src/test/resources/data/output_order.xlsx
+++ b/at_amazon/src/test/resources/data/output_order.xlsx
@@ -12,21 +12,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
   <si>
     <t>IDtc</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>message</t>
-  </si>
-  <si>
-    <t>result</t>
+    <t>Full name</t>
+  </si>
+  <si>
+    <t>Stresst Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Results</t>
   </si>
   <si>
     <t>01</t>
@@ -41,7 +50,16 @@
     <t>Ha Noi</t>
   </si>
   <si>
-    <t>11616</t>
+    <t>100000</t>
+  </si>
+  <si>
+    <t>0879231543</t>
+  </si>
+  <si>
+    <t>Please enter a name.</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
   <si>
     <t>02</t>
@@ -50,13 +68,28 @@
     <t>Ngoc Vu</t>
   </si>
   <si>
+    <t>Please enter an address.</t>
+  </si>
+  <si>
     <t>03</t>
   </si>
   <si>
+    <t>Please enter a ZIP or postal code.</t>
+  </si>
+  <si>
     <t>04</t>
   </si>
   <si>
-    <t>06</t>
+    <t>Please enter a phone number so we can call if there are any issues with delivery.</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>Please provide a valid phone number</t>
   </si>
 </sst>
 </file>
@@ -101,7 +134,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -123,90 +156,144 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
         <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>